<commit_message>
We Have Back Dating
</commit_message>
<xml_diff>
--- a/Backend/output.xlsx
+++ b/Backend/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,70 +446,54 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>GL Code</t>
+          <t>Division</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Plan</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Tier</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Plan</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Tier</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Funding Amount</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Joined</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jane Johnson</t>
+          <t>John Jones</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GL35688</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Carrier1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Tier3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Tier2</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>24.62</t>
+          <t>10418.43</t>
         </is>
       </c>
     </row>
@@ -517,165 +501,71 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Michelle Johnson</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GL78881</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>Carrier2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Tier1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tier2</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>24.62</t>
+          <t>17.63</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Joined</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Alice Brown</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GL38764</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Carrier1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Tier4</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tier2</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>24.62</t>
+          <t>406.38</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mike Doe</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GL44430</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Director</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tier2</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>24.62</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Alex Williams</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GL35279</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tier2</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>24.62</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>123.10</t>
+          <t>10842.44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some modify Methods
</commit_message>
<xml_diff>
--- a/Backend/output.xlsx
+++ b/Backend/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,25 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Admin Fee</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Total Amount</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Dependent Name</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Dependent Tier</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Dependent Relationship</t>
         </is>
@@ -524,73 +534,65 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>51.30</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Casey Smith</t>
+          <t>0.20</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Tier1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Spouse</t>
-        </is>
-      </c>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dependent:</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Jane Johnson</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>GL35688</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Houston</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Director</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Carrier1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>39.00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>9.10</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>48.10</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Casey Smith</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>Tier1</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>51.30</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Casey Smith</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Tier1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Spouse</t>
         </is>
@@ -630,12 +632,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>3.20</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -671,12 +683,22 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>3.20</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -712,12 +734,22 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>3.20</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -753,15 +785,29 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>3.20</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -770,12 +816,22 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>115.40</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+          <t>54.00</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10.10</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>64.10</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>